<commit_message>
Restructured for separate backend
</commit_message>
<xml_diff>
--- a/docs/DBSeedInfo.xlsx
+++ b/docs/DBSeedInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marylark/Desktop/appacademy/CF-Riders/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{500B3595-0AE0-1147-868C-1DD49DF8DBC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547857C4-B4BC-BD46-B469-3D6C7333D3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51700" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{7CB1CEAA-CFF4-A143-8F52-7BBA36256326}"/>
+    <workbookView xWindow="53580" yWindow="1760" windowWidth="28040" windowHeight="17440" xr2:uid="{7CB1CEAA-CFF4-A143-8F52-7BBA36256326}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="111">
   <si>
     <t>Users</t>
   </si>
@@ -183,12 +183,241 @@
   <si>
     <t>Accessories</t>
   </si>
+  <si>
+    <t>GatorskinTire.png</t>
+  </si>
+  <si>
+    <t>Gatorskin Tire Clincher</t>
+  </si>
+  <si>
+    <t>Continental's tried and true all-season tire
+Duraskin sidewalls and durable casing prevent punctures</t>
+  </si>
+  <si>
+    <t>S-WorksPowerSaddle.png</t>
+  </si>
+  <si>
+    <t>S-Works Power Saddle</t>
+  </si>
+  <si>
+    <t>The S-Works series showcases premier cycling gear from Specialized, and the S-Works Power Saddle is the lightest and one of the stiffest saddles out there. Specialized made the shell and rails our of carbon for stiff support at a low weight, and a lab-tested Body Geometry design assures blood flow to sensitive arteries with pressure-mapped, lightweight padding. The saddle's channel is extra wide and elongated to provide bone support and all-day comfort.</t>
+  </si>
+  <si>
+    <t>Fine-tuned for helping you perform at your best, the S-Works Power Saddle features the lightest padding from Specialized, and it still feels supportive on longer rides. A light-but-tough cover protects the padding with reliable water-resistance. The saddle is compatible with SWAT storage devices from Specialized for clever pocketing.</t>
+  </si>
+  <si>
+    <t>WahooElemntBOLTGPS.png</t>
+  </si>
+  <si>
+    <t>Wahoo Elemnt Bolt GPS Bike Computer</t>
+  </si>
+  <si>
+    <t>The ELMNT BOLT is a high-end GPS cycling computer with a unique aerodynamic shape that's been tested and proven to minimize drag at the front of your bicycle. Despite the BOLT's compact aero shape, it tracks and displays more metrics than most riders will ever need—all while remaining simple and intuitive to use. Bluetooth and ANT+ technology allow the BOLT to pair seamlessly with all of your cycling sensors, and the free ELMNT companion app makes it easy to customize your displayed data fields, upload maps and routes, track performance, and share ride data effortlessly. This updated version comes in a new stealth black colorway and features the latest firmware update from Wahoo.</t>
+  </si>
+  <si>
+    <t>DevaBottleCage.png</t>
+  </si>
+  <si>
+    <t>We'll admit it; we love shaving weight off of our bikes. While we haven't been fully diagnosed with the weight weenie syndrome, we absolutely refuse to sacrifice performance or durability in the quest of shedding additional grams.</t>
+  </si>
+  <si>
+    <t>One product that we have had zero reservations about putting on our bike is the Deva Bottle Cage from Tacx. It's constructed from carbon reinforced nylon and weighs an astonishing 32 grams, while its cylindrical shape provides a firm grip on bottles. Blast over railroad tracks and rough country roads without fear of the dreaded bottle ejection. Unlike other cages that promise a vice-like hold, this one has been designed so that the bottle can be inserted and removed easily and smoothly. Trusted by many pro teams, the Diva cage is ready to find a home on your</t>
+  </si>
+  <si>
+    <t>Deva Bottle Cage</t>
+  </si>
+  <si>
+    <t>LezyneRoadDrivePump.png</t>
+  </si>
+  <si>
+    <t>Lezyne Road Drive Pump</t>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lezyne Road Drive Pump</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> is to the Carbon what the Carbon Pressure Drive is to the Pressure Drive. This is the same smart pump design, with the same features, but with one change: CNC-machined aluminum standing in for carbon fiber at the handle, barrel, and frame mount. CNC-machined aluminum remains for the piston and end caps. It's a noticeable savings at the cost of a few grams.</t>
+    </r>
+  </si>
+  <si>
+    <t>As with other Lezyne mini-pumps, this one comes with a hose. In this case, the ABS Speed Hose. This is a huge benefit for a few reasons. One is ergonomics; you aren't limited by holding the pump at a perfect right angle to the valve. A second is that this Flex Hose is ABS-equipped -- it has a bleeder valve on it. Because this is for Presta valves only, the pump head is fitted with a</t>
+  </si>
+  <si>
+    <t>NiteriderLumina.png</t>
+  </si>
+  <si>
+    <t>Niterider Lumina Micro 900 and Sabre 110 Combo</t>
+  </si>
+  <si>
+    <t>Combination lithium headlight with Cree LED bulbs.  Burntime approximately 2h (high), or 60h (flash).  Mounts on the handlebar and seatpost.  Includes rechareable battery, handlebar mount, seatpost strap mount, and 2 USB charging cables.</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>CastelliFullZipJersey.png</t>
+  </si>
+  <si>
+    <t>Castelli Diagonal Full-Zip Jersey - Women's</t>
+  </si>
+  <si>
+    <t>Castelli’s pro-level Diagonal Jersey fills a specific need in the dedicated cyclist’s wardrobe, providing thermal comfort on dry rides ranging from 54-64 degrees F. With warming fabric throughout and a little extra stretch thrown in on the side panels, the jersey is relatively basic in construction compared to the deeper winter layers from Castelli’s vast line up. However, that was the intent as the Diagonal complements Castelli’s range and matches well with its Perfetto or Aria vests on colder rides that need wind-blocking.</t>
+  </si>
+  <si>
+    <t>CastelliFioritaJersey.png</t>
+  </si>
+  <si>
+    <t>Castelli Fiorita Jersey - Women's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front and Back ProSecco Micromesh with Velocity Rev2 sleeves.  Form fit and full length.  Great for Spring, Summer and Fall.  3 rear pockets with Reflective accents.  </t>
+  </si>
+  <si>
+    <t>PearlIzumiQuestJersey.png</t>
+  </si>
+  <si>
+    <t>Pearl Izumi Quest Thermal Jersey - Men's</t>
+  </si>
+  <si>
+    <t>Keep your cool, or rather, warmth, when mother nature hits you with the old 1-2 punch of winter winds and snow by layering up with the right pieces for the cold season. The Quest Thermal Jersey provides ample insulation for diving temperatures, so you can hammer out the miles unhindered by chills.</t>
+  </si>
+  <si>
+    <t>SpecializedCyclingShoe.png</t>
+  </si>
+  <si>
+    <t>Specialized S-Works 7 Cycling Shoe</t>
+  </si>
+  <si>
+    <t>The S-Works 7 series includes the most advanced cycling gear from Specialized, and the Men's S-Works 7 Cycling Shoe strives for perfect road performance without compromising comfort. Made of ply-by-ply carbon originally developed for racing, Powerline is the stiffest, lightest sole from Specialized, and it's fine-tuned for transferring all the power you push down on those pedals with. The upper is made out of Dyneema Mesh trapped between layers of four-way stretch and TPU for malleability in key areas and a formed fit. To provide better connectivity and overall comfort, there's extra room in the toebox, while the PadLock heel counter locks your foot in place for a slip-proof feel.</t>
+  </si>
+  <si>
+    <t>GoreWindstopperGlove.png</t>
+  </si>
+  <si>
+    <t>Gore Wear Windstopper Glove - Men's</t>
+  </si>
+  <si>
+    <t>When weather is unpredictable, reach for gloves that perform no matter the conditions, like the Gore Windstopper Gloves. These gloves offer protection for a slew of activities, with water-resistant and breathable outer shell that cuts through the elements, and pre-shaped fingers to reduce bulk.</t>
+  </si>
+  <si>
+    <t>AssosUMAHalfShort.png</t>
+  </si>
+  <si>
+    <t>ASSOS UMA GT Evo Half Short - Women's</t>
+  </si>
+  <si>
+    <t>Updated and from their predecessor, the UMA GT Evo Half Short proves you can leave the bibs behind and still get the comfort and support you want and need, helping you perform your best on solo efforts or during challenging road races. Features like the revolutionary goldenGate chamois construction method allow the Swiss manufacturer the ability to attach the chamois at the front and rear while leaving the sides free to float with your body instead of against it. This all but eliminates friction from the chamois and shorts eradicating skin irritation in sensitive areas. Imitation is the sincerest form of flattery, and we're seeing similar construction from other manufacturers but Assos is often the one who does it first and continues to do it the best. After all, Assos was the first company to bring a Lycra cycling short to market. The lack of bibs allows these shorts to remain comfortable during warm rides and make stopping for nature breaks a</t>
+  </si>
+  <si>
+    <t>CastelliTalentoSock.png</t>
+  </si>
+  <si>
+    <t>Castelli Talento Sock - Women's</t>
+  </si>
+  <si>
+    <t>Made from Meryl Skinlife, this lightweight road cycling sock sports a 12cm height and a 1 year manufacturer warranty!</t>
+  </si>
+  <si>
+    <t>Bicycle Details</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>frame</t>
+  </si>
+  <si>
+    <t>productId_FK</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>updatedAt</t>
+  </si>
+  <si>
+    <t>52cm</t>
+  </si>
+  <si>
+    <t>5lbs</t>
+  </si>
+  <si>
+    <t>carbon fiber</t>
+  </si>
+  <si>
+    <t>50cm</t>
+  </si>
+  <si>
+    <t>8lbs</t>
+  </si>
+  <si>
+    <t>53cm</t>
+  </si>
+  <si>
+    <t>10lbs</t>
+  </si>
+  <si>
+    <t>aluminum</t>
+  </si>
+  <si>
+    <t>55cm</t>
+  </si>
+  <si>
+    <t>6lbs</t>
+  </si>
+  <si>
+    <t>51cm</t>
+  </si>
+  <si>
+    <t>15lbs</t>
+  </si>
+  <si>
+    <t>Clothing Details</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>productId _FK</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,6 +475,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -279,6 +521,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,17 +836,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FDEC88-54D6-564B-A081-40864019C9B8}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="60" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="239.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -777,6 +1020,429 @@
         <v>41</v>
       </c>
     </row>
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="C30" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="C33" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="C35" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" t="s">
+        <v>88</v>
+      </c>
+      <c r="E50" t="s">
+        <v>89</v>
+      </c>
+      <c r="F50" t="s">
+        <v>91</v>
+      </c>
+      <c r="G50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" t="s">
+        <v>97</v>
+      </c>
+      <c r="E52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>6</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>7</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" t="s">
+        <v>97</v>
+      </c>
+      <c r="E56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>8</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>9</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>103</v>
+      </c>
+      <c r="D58" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>16</v>
+      </c>
+      <c r="C62" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>17</v>
+      </c>
+      <c r="C63" t="s">
+        <v>108</v>
+      </c>
+      <c r="D63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>22</v>
+      </c>
+      <c r="C68" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>